<commit_message>
nieuwe documentatie Kerntaak 2
</commit_message>
<xml_diff>
--- a/DataBase/Normaliseren/Normaliseren.xlsx
+++ b/DataBase/Normaliseren/Normaliseren.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,14 +11,111 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+  <si>
+    <t>Stap 0</t>
+  </si>
+  <si>
+    <t>AreaID</t>
+  </si>
+  <si>
+    <t>AreaName</t>
+  </si>
+  <si>
+    <t>ExtendedDescription</t>
+  </si>
+  <si>
+    <t>BriefDescription</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>BestSeason</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Image1</t>
+  </si>
+  <si>
+    <t>Image2</t>
+  </si>
+  <si>
+    <t>Image3</t>
+  </si>
+  <si>
+    <t>Image4</t>
+  </si>
+  <si>
+    <t>Stap 1</t>
+  </si>
+  <si>
+    <t>Tbl_NatureArea</t>
+  </si>
+  <si>
+    <t>*AreaName</t>
+  </si>
+  <si>
+    <t>*BriefDescription</t>
+  </si>
+  <si>
+    <t>*ExtendedDescription</t>
+  </si>
+  <si>
+    <t>*Latitude</t>
+  </si>
+  <si>
+    <t>*Longitude</t>
+  </si>
+  <si>
+    <t>*Location</t>
+  </si>
+  <si>
+    <t>*BestSeason</t>
+  </si>
+  <si>
+    <t>Tbl_NatureAreaFoto</t>
+  </si>
+  <si>
+    <t>Stap 2</t>
+  </si>
+  <si>
+    <t>N.V.T.</t>
+  </si>
+  <si>
+    <t>Stap 3</t>
+  </si>
+  <si>
+    <t>Tbl_natureAreaFoto</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -34,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -42,25 +139,282 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Rechte verbindingslijn met pijl 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1933575" y="7239000"/>
+          <a:ext cx="47625" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Rechte verbindingslijn met pijl 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1933575" y="7248525"/>
+          <a:ext cx="57150" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Rechte verbindingslijn met pijl 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2714625" y="8867775"/>
+          <a:ext cx="1266825" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Rechte verbindingslijn met pijl 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2705100" y="8858250"/>
+          <a:ext cx="1285875" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +452,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +524,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +697,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>